<commit_message>
Update score prime 2024-2 reference & score data, update score prime admin templates & views
</commit_message>
<xml_diff>
--- a/score/management/commands/data/prime_department.xlsx
+++ b/score/management/commands/data/prime_department.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\score\management\commands\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C85505E-6F39-4B29-95E1-1A8841F08955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B81755A-8EE7-49DD-895D-B3F6355AC0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="19005" windowHeight="16200" tabRatio="645" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="16440" windowHeight="28440" tabRatio="645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exam" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -248,6 +248,14 @@
   </si>
   <si>
     <t>5급공채-기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프라임모의고사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1729,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E962E990-F598-4DE0-9803-142661D1CF89}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1868,7 +1876,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -2448,10 +2467,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70190398-4986-403C-90C2-5314B17F5EE4}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2463,7 +2482,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A1:C8" ca="1">OFFSET(Sheet4!$A$1:$C$1,0,0,COUNTA(Sheet4!$A:$A))</f>
+        <f t="array" aca="1" ref="A1:C9" ca="1">OFFSET(Sheet4!$A$1:$C$1,0,0,COUNTA(Sheet4!$A:$A))</f>
         <v>id</v>
       </c>
       <c r="B1" t="str">
@@ -2571,6 +2590,20 @@
       <c r="C8" t="str">
         <f ca="1"/>
         <v>지역인재 7급</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f ca="1"/>
+        <v>11</v>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1"/>
+        <v>기타</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update score predict views, templates
</commit_message>
<xml_diff>
--- a/score/management/commands/data/prime_department.xlsx
+++ b/score/management/commands/data/prime_department.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\score\management\commands\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B81755A-8EE7-49DD-895D-B3F6355AC0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC7F747-2744-405C-A3E1-8A9A89F59A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="16440" windowHeight="28440" tabRatio="645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1738,7 +1738,7 @@
   <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>